<commit_message>
train AI with new data
</commit_message>
<xml_diff>
--- a/data_19jan/01191532_5x5_b5.xlsx
+++ b/data_19jan/01191532_5x5_b5.xlsx
@@ -1,43 +1,55 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -46,93 +58,56 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
+  <cellXfs count="5">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -141,10 +116,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -182,69 +157,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -268,54 +245,53 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="15000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
+                <a:tint val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -325,7 +301,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -334,7 +310,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -343,7 +319,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -351,10 +327,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -383,7 +359,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -396,13 +372,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
+                <a:tint val="80000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -420,1434 +395,1437 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="n">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+      <c r="A1" s="1">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="n">
+      <c r="B1" s="1">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="C1" s="1">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="D1" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="2">
         <v>0.19</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" s="2">
         <v>1.26</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" s="2">
         <v>1.41</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" s="2">
         <v>1.33</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+      <c r="A3" s="2">
         <v>0.16</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="2">
         <v>1.1</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" s="2">
         <v>0.61</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+      <c r="A4" s="2">
         <v>0.38</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" s="2">
         <v>1.85</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" s="2">
         <v>0.84</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" s="2">
         <v>1.78</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+      <c r="A5" s="2">
         <v>0.12</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" s="2">
         <v>1.41</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" s="2">
         <v>0.79</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5" s="2">
         <v>1.29</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="B6" t="n">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+      <c r="A6" s="2">
+        <v>0.07</v>
+      </c>
+      <c r="B6" s="2">
         <v>0.84</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" s="2">
         <v>0.61</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6" s="2">
         <v>0.89</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+      <c r="A7" s="2">
         <v>0.25</v>
       </c>
-      <c r="B7" t="n">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="C7" t="n">
+      <c r="B7" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="C7" s="2">
         <v>0.78</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7" s="2">
         <v>0.98</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+      <c r="A8" s="2">
         <v>0.23</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" s="2">
         <v>1.69</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8" s="2">
         <v>0.47</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8" s="2">
         <v>0.87</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="n">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+      <c r="A9" s="2">
         <v>0.09</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9" s="2">
         <v>1.54</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9" s="2">
         <v>1.1</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9" s="2">
         <v>0.89</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="n">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+      <c r="A10" s="2">
         <v>0.1</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10" s="2">
         <v>2.37</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10" s="2">
         <v>0.89</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10" s="2">
         <v>0.95</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="n">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+      <c r="A11" s="2">
         <v>0.23</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11" s="2">
         <v>1.59</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11" s="2">
         <v>0.57</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11" s="2">
         <v>1.06</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="n">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+      <c r="A12" s="2">
         <v>0.21</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12" s="2">
         <v>1.33</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12" s="2">
         <v>1.42</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D12" s="2">
         <v>1.64</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="n">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+      <c r="A13" s="2">
         <v>0.17</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13" s="2">
         <v>1.63</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13" s="2">
         <v>0.62</v>
       </c>
-      <c r="D13" t="n">
+      <c r="D13" s="2">
         <v>1.02</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="n">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+      <c r="A14" s="2">
         <v>0.33</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14" s="2">
         <v>1.27</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C14" s="2">
         <v>0.95</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D14" s="2">
         <v>1.12</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="n">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+      <c r="A15" s="2">
         <v>0.12</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15" s="2">
         <v>1.63</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15" s="2">
         <v>0.97</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D15" s="2">
         <v>1.81</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="n">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+      <c r="A16" s="2">
         <v>0.06</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16" s="2">
         <v>0.92</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C16" s="2">
         <v>0.58</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D16" s="2">
         <v>0.89</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="n">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+      <c r="A17" s="2">
         <v>0.22</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17" s="2">
         <v>0.78</v>
       </c>
-      <c r="C17" t="n">
-        <v>0.8100000000000001</v>
-      </c>
-      <c r="D17" t="n">
+      <c r="C17" s="2">
+        <v>0.81</v>
+      </c>
+      <c r="D17" s="2">
         <v>0.88</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="n">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+      <c r="A18" s="2">
         <v>0.23</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B18" s="2">
         <v>1.9</v>
       </c>
-      <c r="C18" t="n">
+      <c r="C18" s="2">
         <v>0.47</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D18" s="2">
         <v>1.05</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="n">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+      <c r="A19" s="2">
         <v>0.1</v>
       </c>
-      <c r="B19" t="n">
+      <c r="B19" s="2">
         <v>1.3</v>
       </c>
-      <c r="C19" t="n">
+      <c r="C19" s="2">
         <v>1.06</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D19" s="2">
         <v>1.24</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="n">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+      <c r="A20" s="2">
         <v>0.09</v>
       </c>
-      <c r="B20" t="n">
+      <c r="B20" s="2">
         <v>1.68</v>
       </c>
-      <c r="C20" t="n">
+      <c r="C20" s="2">
         <v>1.09</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D20" s="2">
         <v>1.15</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="n">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+      <c r="A21" s="2">
         <v>0.21</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21" s="2">
         <v>1.12</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C21" s="2">
         <v>0.61</v>
       </c>
-      <c r="D21" t="n">
+      <c r="D21" s="2">
         <v>1.25</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="n">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+      <c r="A22" s="2">
         <v>0.2</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22" s="2">
         <v>1.13</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C22" s="2">
         <v>0.86</v>
       </c>
-      <c r="D22" t="n">
+      <c r="D22" s="2">
         <v>1.5</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="n">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+      <c r="A23" s="2">
         <v>0.16</v>
       </c>
-      <c r="B23" t="n">
+      <c r="B23" s="2">
         <v>1.88</v>
       </c>
-      <c r="C23" t="n">
+      <c r="C23" s="2">
         <v>0.64</v>
       </c>
-      <c r="D23" t="n">
+      <c r="D23" s="2">
         <v>1.09</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="n">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+      <c r="A24" s="2">
         <v>0.4</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24" s="2">
         <v>1.78</v>
       </c>
-      <c r="C24" t="n">
+      <c r="C24" s="2">
         <v>1.26</v>
       </c>
-      <c r="D24" t="n">
+      <c r="D24" s="2">
         <v>1.34</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="n">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+      <c r="A25" s="2">
         <v>0.12</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B25" s="2">
         <v>1.5</v>
       </c>
-      <c r="C25" t="n">
+      <c r="C25" s="2">
         <v>0.79</v>
       </c>
-      <c r="D25" t="n">
+      <c r="D25" s="2">
         <v>1.33</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="B26" t="n">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+      <c r="A26" s="2">
+        <v>0.07</v>
+      </c>
+      <c r="B26" s="2">
         <v>0.82</v>
       </c>
-      <c r="C26" t="n">
+      <c r="C26" s="2">
         <v>0.71</v>
       </c>
-      <c r="D26" t="n">
+      <c r="D26" s="2">
         <v>0.89</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="n">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+      <c r="A27" s="2">
         <v>0.25</v>
       </c>
-      <c r="B27" t="n">
+      <c r="B27" s="2">
         <v>0.91</v>
       </c>
-      <c r="C27" t="n">
+      <c r="C27" s="2">
         <v>0.8</v>
       </c>
-      <c r="D27" t="n">
+      <c r="D27" s="2">
         <v>0.96</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="n">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
+      <c r="A28" s="2">
         <v>0.23</v>
       </c>
-      <c r="B28" t="n">
+      <c r="B28" s="2">
         <v>1.46</v>
       </c>
-      <c r="C28" t="n">
+      <c r="C28" s="2">
         <v>0.48</v>
       </c>
-      <c r="D28" t="n">
+      <c r="D28" s="2">
         <v>1.06</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="n">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
+      <c r="A29" s="2">
         <v>0.09</v>
       </c>
-      <c r="B29" t="n">
+      <c r="B29" s="2">
         <v>1.78</v>
       </c>
-      <c r="C29" t="n">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="D29" t="n">
+      <c r="C29" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="D29" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="n">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
+      <c r="A30" s="2">
         <v>0.1</v>
       </c>
-      <c r="B30" t="n">
+      <c r="B30" s="2">
         <v>2.25</v>
       </c>
-      <c r="C30" t="n">
+      <c r="C30" s="2">
         <v>1.11</v>
       </c>
-      <c r="D30" t="n">
+      <c r="D30" s="2">
         <v>0.93</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="n">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
+      <c r="A31" s="2">
         <v>0.22</v>
       </c>
-      <c r="B31" t="n">
+      <c r="B31" s="2">
         <v>1.35</v>
       </c>
-      <c r="C31" t="n">
+      <c r="C31" s="2">
         <v>0.58</v>
       </c>
-      <c r="D31" t="n">
+      <c r="D31" s="2">
         <v>0.84</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="n">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
+      <c r="A32" s="2">
         <v>0.2</v>
       </c>
-      <c r="B32" t="n">
+      <c r="B32" s="2">
         <v>1.31</v>
       </c>
-      <c r="C32" t="n">
+      <c r="C32" s="2">
         <v>1.62</v>
       </c>
-      <c r="D32" t="n">
+      <c r="D32" s="2">
         <v>1.47</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="n">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
+      <c r="A33" s="2">
         <v>0.17</v>
       </c>
-      <c r="B33" t="n">
+      <c r="B33" s="2">
         <v>1.19</v>
       </c>
-      <c r="C33" t="n">
+      <c r="C33" s="2">
         <v>0.62</v>
       </c>
-      <c r="D33" t="n">
+      <c r="D33" s="2">
         <v>0.89</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" t="n">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
+      <c r="A34" s="2">
         <v>0.53</v>
       </c>
-      <c r="B34" t="n">
+      <c r="B34" s="2">
         <v>1.61</v>
       </c>
-      <c r="C34" t="n">
+      <c r="C34" s="2">
         <v>1.78</v>
       </c>
-      <c r="D34" t="n">
+      <c r="D34" s="2">
         <v>1.28</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="n">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
+      <c r="A35" s="2">
         <v>0.13</v>
       </c>
-      <c r="B35" t="n">
+      <c r="B35" s="2">
         <v>1.68</v>
       </c>
-      <c r="C35" t="n">
+      <c r="C35" s="2">
         <v>0.75</v>
       </c>
-      <c r="D35" t="n">
+      <c r="D35" s="2">
         <v>1.4</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="B36" t="n">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
+      <c r="A36" s="2">
+        <v>0.07</v>
+      </c>
+      <c r="B36" s="2">
         <v>0.85</v>
       </c>
-      <c r="C36" t="n">
+      <c r="C36" s="2">
         <v>0.65</v>
       </c>
-      <c r="D36" t="n">
+      <c r="D36" s="2">
         <v>0.83</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="n">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
+      <c r="A37" s="2">
         <v>0.24</v>
       </c>
-      <c r="B37" t="n">
+      <c r="B37" s="2">
         <v>0.8</v>
       </c>
-      <c r="C37" t="n">
+      <c r="C37" s="2">
         <v>0.72</v>
       </c>
-      <c r="D37" t="n">
+      <c r="D37" s="2">
         <v>0.92</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" t="n">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
+      <c r="A38" s="2">
         <v>0.32</v>
       </c>
-      <c r="B38" t="n">
+      <c r="B38" s="2">
         <v>1.89</v>
       </c>
-      <c r="C38" t="n">
+      <c r="C38" s="2">
         <v>0.47</v>
       </c>
-      <c r="D38" t="n">
+      <c r="D38" s="2">
         <v>0.97</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="n">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
+      <c r="A39" s="2">
         <v>0.1</v>
       </c>
-      <c r="B39" t="n">
+      <c r="B39" s="2">
         <v>1.52</v>
       </c>
-      <c r="C39" t="n">
+      <c r="C39" s="2">
         <v>0.79</v>
       </c>
-      <c r="D39" t="n">
+      <c r="D39" s="2">
         <v>0.92</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" t="n">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
+      <c r="A40" s="2">
         <v>0.09</v>
       </c>
-      <c r="B40" t="n">
+      <c r="B40" s="2">
         <v>1.68</v>
       </c>
-      <c r="C40" t="n">
+      <c r="C40" s="3">
         <v>0</v>
       </c>
-      <c r="D40" t="n">
+      <c r="D40" s="2">
         <v>1.09</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="n">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
+      <c r="A41" s="2">
         <v>0.22</v>
       </c>
-      <c r="B41" t="n">
+      <c r="B41" s="2">
         <v>1.16</v>
       </c>
-      <c r="C41" t="n">
+      <c r="C41" s="2">
         <v>0.67</v>
       </c>
-      <c r="D41" t="n">
+      <c r="D41" s="2">
         <v>1.21</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="n">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25">
+      <c r="A42" s="2">
         <v>0.19</v>
       </c>
-      <c r="B42" t="n">
+      <c r="B42" s="2">
         <v>1.27</v>
       </c>
-      <c r="C42" t="n">
+      <c r="C42" s="2">
         <v>1.32</v>
       </c>
-      <c r="D42" t="n">
+      <c r="D42" s="2">
         <v>1.58</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" t="n">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25">
+      <c r="A43" s="2">
         <v>0.16</v>
       </c>
-      <c r="B43" t="n">
+      <c r="B43" s="2">
         <v>1.24</v>
       </c>
-      <c r="C43" t="n">
+      <c r="C43" s="2">
         <v>0.63</v>
       </c>
-      <c r="D43" t="n">
+      <c r="D43" s="2">
         <v>1.03</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="n">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25">
+      <c r="A44" s="2">
         <v>0.37</v>
       </c>
-      <c r="B44" t="n">
+      <c r="B44" s="2">
         <v>1.19</v>
       </c>
-      <c r="C44" t="n">
+      <c r="C44" s="2">
         <v>1.01</v>
       </c>
-      <c r="D44" t="n">
+      <c r="D44" s="2">
         <v>0.77</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" t="n">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25">
+      <c r="A45" s="2">
         <v>0.12</v>
       </c>
-      <c r="B45" t="n">
+      <c r="B45" s="2">
         <v>1.58</v>
       </c>
-      <c r="C45" t="n">
+      <c r="C45" s="2">
         <v>0.92</v>
       </c>
-      <c r="D45" t="n">
+      <c r="D45" s="2">
         <v>1.46</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="B46" t="n">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25">
+      <c r="A46" s="2">
+        <v>0.07</v>
+      </c>
+      <c r="B46" s="2">
         <v>0.84</v>
       </c>
-      <c r="C46" t="n">
+      <c r="C46" s="2">
         <v>0.58</v>
       </c>
-      <c r="D46" t="n">
+      <c r="D46" s="2">
         <v>0.91</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" t="n">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25">
+      <c r="A47" s="2">
         <v>0.21</v>
       </c>
-      <c r="B47" t="n">
+      <c r="B47" s="2">
         <v>0.89</v>
       </c>
-      <c r="C47" t="n">
+      <c r="C47" s="2">
         <v>0.84</v>
       </c>
-      <c r="D47" t="n">
+      <c r="D47" s="2">
         <v>1.03</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" t="n">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25">
+      <c r="A48" s="2">
         <v>0.24</v>
       </c>
-      <c r="B48" t="n">
+      <c r="B48" s="3">
         <v>0</v>
       </c>
-      <c r="C48" t="n">
+      <c r="C48" s="2">
         <v>0.45</v>
       </c>
-      <c r="D48" t="n">
+      <c r="D48" s="2">
         <v>0.89</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" t="n">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25">
+      <c r="A49" s="2">
         <v>0.09</v>
       </c>
-      <c r="B49" t="n">
+      <c r="B49" s="2">
         <v>1.47</v>
       </c>
-      <c r="C49" t="n">
+      <c r="C49" s="3">
         <v>1</v>
       </c>
-      <c r="D49" t="n">
+      <c r="D49" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" t="n">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="17.25">
+      <c r="A50" s="2">
         <v>0.1</v>
       </c>
-      <c r="B50" t="n">
+      <c r="B50" s="2">
         <v>2.51</v>
       </c>
-      <c r="C50" t="n">
+      <c r="C50" s="2">
         <v>1.06</v>
       </c>
-      <c r="D50" t="n">
+      <c r="D50" s="2">
         <v>0.84</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" t="n">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="17.25">
+      <c r="A51" s="2">
         <v>0.21</v>
       </c>
-      <c r="B51" t="n">
+      <c r="B51" s="2">
         <v>1.72</v>
       </c>
-      <c r="C51" t="n">
+      <c r="C51" s="2">
         <v>0.54</v>
       </c>
-      <c r="D51" t="n">
+      <c r="D51" s="2">
         <v>1.15</v>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" t="n">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="17.25">
+      <c r="A52" s="2">
         <v>0.19</v>
       </c>
-      <c r="B52" t="n">
+      <c r="B52" s="2">
         <v>1.17</v>
       </c>
-      <c r="C52" t="n">
+      <c r="C52" s="2">
         <v>0.95</v>
       </c>
-      <c r="D52" t="n">
+      <c r="D52" s="2">
         <v>1.65</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" t="n">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="17.25">
+      <c r="A53" s="2">
         <v>0.17</v>
       </c>
-      <c r="B53" t="n">
+      <c r="B53" s="2">
         <v>1.45</v>
       </c>
-      <c r="C53" t="n">
+      <c r="C53" s="2">
         <v>0.6</v>
       </c>
-      <c r="D53" t="n">
+      <c r="D53" s="2">
         <v>0.96</v>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" t="n">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="17.25">
+      <c r="A54" s="2">
         <v>0.3</v>
       </c>
-      <c r="B54" t="n">
+      <c r="B54" s="2">
         <v>1.41</v>
       </c>
-      <c r="C54" t="n">
+      <c r="C54" s="2">
         <v>0.86</v>
       </c>
-      <c r="D54" t="n">
+      <c r="D54" s="2">
         <v>1.43</v>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" t="n">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="17.25">
+      <c r="A55" s="2">
         <v>0.13</v>
       </c>
-      <c r="B55" t="n">
+      <c r="B55" s="2">
         <v>1.65</v>
       </c>
-      <c r="C55" t="n">
+      <c r="C55" s="2">
         <v>1.03</v>
       </c>
-      <c r="D55" t="n">
+      <c r="D55" s="2">
         <v>1.85</v>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="B56" t="n">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="C56" t="n">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="D56" t="n">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="17.25">
+      <c r="A56" s="2">
+        <v>0.07</v>
+      </c>
+      <c r="B56" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="C56" s="2">
+        <v>0.56</v>
+      </c>
+      <c r="D56" s="2">
         <v>0.89</v>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" t="n">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="17.25">
+      <c r="A57" s="2">
         <v>0.22</v>
       </c>
-      <c r="B57" t="n">
+      <c r="B57" s="2">
         <v>0.8</v>
       </c>
-      <c r="C57" t="n">
+      <c r="C57" s="2">
         <v>0.78</v>
       </c>
-      <c r="D57" t="n">
+      <c r="D57" s="2">
         <v>0.91</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" t="n">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="17.25">
+      <c r="A58" s="2">
         <v>0.22</v>
       </c>
-      <c r="B58" t="n">
+      <c r="B58" s="2">
         <v>1.72</v>
       </c>
-      <c r="C58" t="n">
+      <c r="C58" s="2">
         <v>0.47</v>
       </c>
-      <c r="D58" t="n">
+      <c r="D58" s="2">
         <v>1.09</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" t="n">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="17.25">
+      <c r="A59" s="2">
         <v>0.1</v>
       </c>
-      <c r="B59" t="n">
+      <c r="B59" s="2">
         <v>1.57</v>
       </c>
-      <c r="C59" t="n">
+      <c r="C59" s="2">
         <v>1.04</v>
       </c>
-      <c r="D59" t="n">
+      <c r="D59" s="2">
         <v>0.84</v>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" t="n">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="17.25">
+      <c r="A60" s="2">
         <v>0.09</v>
       </c>
-      <c r="B60" t="n">
+      <c r="B60" s="2">
         <v>1.88</v>
       </c>
-      <c r="C60" t="n">
+      <c r="C60" s="2">
         <v>1.12</v>
       </c>
-      <c r="D60" t="n">
+      <c r="D60" s="2">
         <v>1.06</v>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" t="n">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="17.25">
+      <c r="A61" s="2">
         <v>0.23</v>
       </c>
-      <c r="B61" t="n">
+      <c r="B61" s="2">
         <v>1.76</v>
       </c>
-      <c r="C61" t="n">
+      <c r="C61" s="2">
         <v>0.53</v>
       </c>
-      <c r="D61" t="n">
+      <c r="D61" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" t="n">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="17.25">
+      <c r="A62" s="2">
         <v>0.19</v>
       </c>
-      <c r="B62" t="n">
+      <c r="B62" s="2">
         <v>1.15</v>
       </c>
-      <c r="C62" t="n">
+      <c r="C62" s="2">
         <v>1.68</v>
       </c>
-      <c r="D62" t="n">
+      <c r="D62" s="2">
         <v>1.41</v>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" t="n">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="17.25">
+      <c r="A63" s="2">
         <v>0.16</v>
       </c>
-      <c r="B63" t="n">
+      <c r="B63" s="2">
         <v>0.95</v>
       </c>
-      <c r="C63" t="n">
+      <c r="C63" s="2">
         <v>0.64</v>
       </c>
-      <c r="D63" t="n">
+      <c r="D63" s="2">
         <v>1.29</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" t="n">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="17.25">
+      <c r="A64" s="2">
         <v>0.33</v>
       </c>
-      <c r="B64" t="n">
+      <c r="B64" s="2">
         <v>1.29</v>
       </c>
-      <c r="C64" t="n">
+      <c r="C64" s="2">
         <v>1.03</v>
       </c>
-      <c r="D64" t="n">
+      <c r="D64" s="2">
         <v>0.91</v>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" t="n">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="17.25">
+      <c r="A65" s="2">
         <v>0.12</v>
       </c>
-      <c r="B65" t="n">
+      <c r="B65" s="2">
         <v>1.66</v>
       </c>
-      <c r="C65" t="n">
+      <c r="C65" s="2">
         <v>1.26</v>
       </c>
-      <c r="D65" t="n">
+      <c r="D65" s="2">
         <v>1.67</v>
       </c>
     </row>
-    <row r="66">
-      <c r="A66" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="B66" t="n">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="C66" t="n">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="17.25">
+      <c r="A66" s="2">
+        <v>0.07</v>
+      </c>
+      <c r="B66" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="C66" s="2">
         <v>0.61</v>
       </c>
-      <c r="D66" t="n">
-        <v>0.9399999999999999</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="n">
+      <c r="D66" s="2">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="17.25">
+      <c r="A67" s="2">
         <v>0.23</v>
       </c>
-      <c r="B67" t="n">
+      <c r="B67" s="2">
         <v>0.78</v>
       </c>
-      <c r="C67" t="n">
+      <c r="C67" s="2">
         <v>0.79</v>
       </c>
-      <c r="D67" t="n">
+      <c r="D67" s="2">
         <v>0.88</v>
       </c>
     </row>
-    <row r="68">
-      <c r="A68" t="n">
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="17.25">
+      <c r="A68" s="2">
         <v>0.18</v>
       </c>
-      <c r="B68" t="n">
+      <c r="B68" s="2">
         <v>1.33</v>
       </c>
-      <c r="C68" t="n">
+      <c r="C68" s="2">
         <v>0.47</v>
       </c>
-      <c r="D68" t="n">
+      <c r="D68" s="2">
         <v>0.91</v>
       </c>
     </row>
-    <row r="69">
-      <c r="A69" t="n">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="17.25">
+      <c r="A69" s="2">
         <v>0.09</v>
       </c>
-      <c r="B69" t="n">
+      <c r="B69" s="2">
         <v>1.31</v>
       </c>
-      <c r="C69" t="n">
+      <c r="C69" s="2">
         <v>0.88</v>
       </c>
-      <c r="D69" t="n">
+      <c r="D69" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" t="n">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="17.25">
+      <c r="A70" s="2">
         <v>0.09</v>
       </c>
-      <c r="B70" t="n">
+      <c r="B70" s="2">
         <v>2.22</v>
       </c>
-      <c r="C70" t="n">
+      <c r="C70" s="2">
         <v>1.23</v>
       </c>
-      <c r="D70" t="n">
+      <c r="D70" s="2">
         <v>1.01</v>
       </c>
     </row>
-    <row r="71">
-      <c r="A71" t="n">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="17.25">
+      <c r="A71" s="2">
         <v>0.22</v>
       </c>
-      <c r="B71" t="n">
+      <c r="B71" s="2">
         <v>1.15</v>
       </c>
-      <c r="C71" t="n">
+      <c r="C71" s="2">
         <v>0.55</v>
       </c>
-      <c r="D71" t="n">
+      <c r="D71" s="2">
         <v>1.14</v>
       </c>
     </row>
-    <row r="72">
-      <c r="A72" t="n">
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="17.25">
+      <c r="A72" s="2">
         <v>0.22</v>
       </c>
-      <c r="B72" t="n">
+      <c r="B72" s="2">
         <v>1.22</v>
       </c>
-      <c r="C72" t="n">
+      <c r="C72" s="2">
         <v>0.9</v>
       </c>
-      <c r="D72" t="n">
+      <c r="D72" s="2">
         <v>1.53</v>
       </c>
     </row>
-    <row r="73">
-      <c r="A73" t="n">
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="17.25">
+      <c r="A73" s="2">
         <v>1.76</v>
       </c>
-      <c r="B73" t="n">
+      <c r="B73" s="2">
         <v>1.35</v>
       </c>
-      <c r="C73" t="n">
+      <c r="C73" s="2">
         <v>0.58</v>
       </c>
-      <c r="D73" t="n">
+      <c r="D73" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" t="n">
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="17.25">
+      <c r="A74" s="2">
         <v>0.3</v>
       </c>
-      <c r="B74" t="n">
+      <c r="B74" s="2">
         <v>1.85</v>
       </c>
-      <c r="C74" t="n">
+      <c r="C74" s="2">
         <v>0.89</v>
       </c>
-      <c r="D74" t="n">
+      <c r="D74" s="2">
         <v>1.45</v>
       </c>
     </row>
-    <row r="75">
-      <c r="A75" t="n">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="17.25">
+      <c r="A75" s="2">
         <v>0.12</v>
       </c>
-      <c r="B75" t="n">
+      <c r="B75" s="2">
         <v>1.79</v>
       </c>
-      <c r="C75" t="n">
+      <c r="C75" s="2">
         <v>0.77</v>
       </c>
-      <c r="D75" t="n">
+      <c r="D75" s="2">
         <v>1.68</v>
       </c>
     </row>
-    <row r="76">
-      <c r="A76" t="n">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="17.25">
+      <c r="A76" s="2">
         <v>0.06</v>
       </c>
-      <c r="B76" t="n">
+      <c r="B76" s="2">
         <v>0.92</v>
       </c>
-      <c r="C76" t="n">
+      <c r="C76" s="2">
         <v>0.6</v>
       </c>
-      <c r="D76" t="n">
+      <c r="D76" s="2">
         <v>0.88</v>
       </c>
     </row>
-    <row r="77">
-      <c r="A77" t="n">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="17.25">
+      <c r="A77" s="2">
         <v>0.23</v>
       </c>
-      <c r="B77" t="n">
+      <c r="B77" s="2">
         <v>0.76</v>
       </c>
-      <c r="C77" t="n">
+      <c r="C77" s="2">
         <v>0.73</v>
       </c>
-      <c r="D77" t="n">
+      <c r="D77" s="2">
         <v>0.99</v>
       </c>
     </row>
-    <row r="78">
-      <c r="A78" t="n">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="17.25">
+      <c r="A78" s="2">
         <v>0.24</v>
       </c>
-      <c r="B78" t="n">
+      <c r="B78" s="2">
         <v>1.66</v>
       </c>
-      <c r="C78" t="n">
+      <c r="C78" s="2">
         <v>0.46</v>
       </c>
-      <c r="D78" t="n">
+      <c r="D78" s="2">
         <v>1.03</v>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" t="n">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="17.25">
+      <c r="A79" s="2">
         <v>0.1</v>
       </c>
-      <c r="B79" t="n">
+      <c r="B79" s="2">
         <v>1.44</v>
       </c>
-      <c r="C79" t="n">
+      <c r="C79" s="2">
         <v>1.18</v>
       </c>
-      <c r="D79" t="n">
+      <c r="D79" s="2">
         <v>0.95</v>
       </c>
     </row>
-    <row r="80">
-      <c r="A80" t="n">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="17.25">
+      <c r="A80" s="2">
         <v>0.09</v>
       </c>
-      <c r="B80" t="n">
+      <c r="B80" s="2">
         <v>2.11</v>
       </c>
-      <c r="C80" t="n">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="D80" t="n">
+      <c r="C80" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="D80" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="81">
-      <c r="A81" t="n">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="17.25">
+      <c r="A81" s="2">
         <v>0.25</v>
       </c>
-      <c r="B81" t="n">
+      <c r="B81" s="2">
         <v>0.89</v>
       </c>
-      <c r="C81" t="n">
+      <c r="C81" s="2">
         <v>0.54</v>
       </c>
-      <c r="D81" t="n">
+      <c r="D81" s="2">
         <v>0.84</v>
       </c>
     </row>
-    <row r="82">
-      <c r="A82" t="n">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="17.25">
+      <c r="A82" s="2">
         <v>0.19</v>
       </c>
-      <c r="B82" t="n">
+      <c r="B82" s="2">
         <v>1.33</v>
       </c>
-      <c r="C82" t="n">
+      <c r="C82" s="2">
         <v>1.59</v>
       </c>
-      <c r="D82" t="n">
+      <c r="D82" s="2">
         <v>1.54</v>
       </c>
     </row>
-    <row r="83">
-      <c r="A83" t="n">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="17.25">
+      <c r="A83" s="2">
         <v>0.16</v>
       </c>
-      <c r="B83" t="n">
+      <c r="B83" s="2">
         <v>1.03</v>
       </c>
-      <c r="C83" t="n">
+      <c r="C83" s="2">
         <v>0.61</v>
       </c>
-      <c r="D83" t="n">
+      <c r="D83" s="2">
         <v>1.38</v>
       </c>
     </row>
-    <row r="84">
-      <c r="A84" t="n">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="17.25">
+      <c r="A84" s="2">
         <v>0.37</v>
       </c>
-      <c r="B84" t="n">
+      <c r="B84" s="2">
         <v>1.19</v>
       </c>
-      <c r="C84" t="n">
+      <c r="C84" s="2">
         <v>0.95</v>
       </c>
-      <c r="D84" t="n">
+      <c r="D84" s="2">
         <v>0.93</v>
       </c>
     </row>
-    <row r="85">
-      <c r="A85" t="n">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="17.25">
+      <c r="A85" s="2">
         <v>0.12</v>
       </c>
-      <c r="B85" t="n">
+      <c r="B85" s="2">
         <v>1.51</v>
       </c>
-      <c r="C85" t="n">
+      <c r="C85" s="2">
         <v>0.89</v>
       </c>
-      <c r="D85" t="n">
+      <c r="D85" s="2">
         <v>1.52</v>
       </c>
     </row>
-    <row r="86">
-      <c r="A86" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="B86" t="n">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="17.25">
+      <c r="A86" s="2">
+        <v>0.07</v>
+      </c>
+      <c r="B86" s="2">
         <v>0.98</v>
       </c>
-      <c r="C86" t="n">
+      <c r="C86" s="2">
         <v>0.57</v>
       </c>
-      <c r="D86" t="n">
+      <c r="D86" s="2">
         <v>0.8</v>
       </c>
     </row>
-    <row r="87">
-      <c r="A87" t="n">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="17.25">
+      <c r="A87" s="2">
         <v>0.22</v>
       </c>
-      <c r="B87" t="n">
+      <c r="B87" s="2">
         <v>0.73</v>
       </c>
-      <c r="C87" t="n">
+      <c r="C87" s="2">
         <v>0.82</v>
       </c>
-      <c r="D87" t="n">
+      <c r="D87" s="2">
         <v>0.9</v>
       </c>
     </row>
-    <row r="88">
-      <c r="A88" t="n">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="17.25">
+      <c r="A88" s="2">
         <v>0.2</v>
       </c>
-      <c r="B88" t="n">
+      <c r="B88" s="2">
         <v>2.11</v>
       </c>
-      <c r="C88" t="n">
+      <c r="C88" s="2">
         <v>0.47</v>
       </c>
-      <c r="D88" t="n">
+      <c r="D88" s="2">
         <v>0.89</v>
       </c>
     </row>
-    <row r="89">
-      <c r="A89" t="n">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="17.25">
+      <c r="A89" s="2">
         <v>0.09</v>
       </c>
-      <c r="B89" t="n">
+      <c r="B89" s="2">
         <v>1.26</v>
       </c>
-      <c r="C89" t="n">
+      <c r="C89" s="2">
         <v>0.89</v>
       </c>
-      <c r="D89" t="n">
-        <v>0.9399999999999999</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="n">
+      <c r="D89" s="2">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="17.25">
+      <c r="A90" s="2">
         <v>0.1</v>
       </c>
-      <c r="B90" t="n">
+      <c r="B90" s="2">
         <v>1.68</v>
       </c>
-      <c r="C90" t="n">
+      <c r="C90" s="2">
         <v>1.19</v>
       </c>
-      <c r="D90" t="n">
+      <c r="D90" s="2">
         <v>1.03</v>
       </c>
     </row>
-    <row r="91">
-      <c r="A91" t="n">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="17.25">
+      <c r="A91" s="2">
         <v>0.22</v>
       </c>
-      <c r="B91" t="n">
+      <c r="B91" s="2">
         <v>1.13</v>
       </c>
-      <c r="C91" t="n">
+      <c r="C91" s="2">
         <v>0.57</v>
       </c>
-      <c r="D91" t="n">
+      <c r="D91" s="2">
         <v>1.01</v>
       </c>
     </row>
-    <row r="92">
-      <c r="A92" t="n">
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="17.25">
+      <c r="A92" s="2">
         <v>0.2</v>
       </c>
-      <c r="B92" t="n">
+      <c r="B92" s="2">
         <v>1.11</v>
       </c>
-      <c r="C92" t="n">
+      <c r="C92" s="2">
         <v>1.28</v>
       </c>
-      <c r="D92" t="n">
+      <c r="D92" s="2">
         <v>1.59</v>
       </c>
     </row>
-    <row r="93">
-      <c r="A93" t="n">
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="17.25">
+      <c r="A93" s="2">
         <v>0.16</v>
       </c>
-      <c r="B93" t="n">
+      <c r="B93" s="2">
         <v>1.23</v>
       </c>
-      <c r="C93" t="n">
+      <c r="C93" s="2">
         <v>0.6</v>
       </c>
-      <c r="D93" t="n">
+      <c r="D93" s="2">
         <v>1.34</v>
       </c>
     </row>
-    <row r="94">
-      <c r="A94" t="n">
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="17.25">
+      <c r="A94" s="2">
         <v>0.31</v>
       </c>
-      <c r="B94" t="n">
+      <c r="B94" s="2">
         <v>1.68</v>
       </c>
-      <c r="C94" t="n">
+      <c r="C94" s="2">
         <v>1.23</v>
       </c>
-      <c r="D94" t="n">
+      <c r="D94" s="2">
         <v>1.12</v>
       </c>
     </row>
-    <row r="95">
-      <c r="A95" t="n">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="17.25">
+      <c r="A95" s="2">
         <v>0.12</v>
       </c>
-      <c r="B95" t="n">
+      <c r="B95" s="2">
         <v>1.58</v>
       </c>
-      <c r="C95" t="n">
+      <c r="C95" s="2">
         <v>0.92</v>
       </c>
-      <c r="D95" t="n">
+      <c r="D95" s="2">
         <v>1.69</v>
       </c>
     </row>
-    <row r="96">
-      <c r="A96" t="n">
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="17.25">
+      <c r="A96" s="2">
         <v>0.06</v>
       </c>
-      <c r="B96" t="n">
+      <c r="B96" s="2">
         <v>0.85</v>
       </c>
-      <c r="C96" t="n">
+      <c r="C96" s="2">
         <v>0.63</v>
       </c>
-      <c r="D96" t="n">
+      <c r="D96" s="2">
         <v>0.89</v>
       </c>
     </row>
-    <row r="97">
-      <c r="A97" t="n">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="17.25">
+      <c r="A97" s="2">
         <v>0.25</v>
       </c>
-      <c r="B97" t="n">
+      <c r="B97" s="2">
         <v>0.89</v>
       </c>
-      <c r="C97" t="n">
-        <v>0.8100000000000001</v>
-      </c>
-      <c r="D97" t="n">
+      <c r="C97" s="2">
+        <v>0.81</v>
+      </c>
+      <c r="D97" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="98">
-      <c r="A98" t="n">
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="17.25">
+      <c r="A98" s="2">
         <v>0.23</v>
       </c>
-      <c r="B98" t="n">
+      <c r="B98" s="2">
         <v>1.65</v>
       </c>
-      <c r="C98" t="n">
+      <c r="C98" s="2">
         <v>0.43</v>
       </c>
-      <c r="D98" t="n">
+      <c r="D98" s="2">
         <v>1.04</v>
       </c>
     </row>
-    <row r="99">
-      <c r="A99" t="n">
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="17.25">
+      <c r="A99" s="2">
         <v>0.1</v>
       </c>
-      <c r="B99" t="n">
+      <c r="B99" s="2">
         <v>1.48</v>
       </c>
-      <c r="C99" t="n">
+      <c r="C99" s="3">
         <v>0</v>
       </c>
-      <c r="D99" t="n">
+      <c r="D99" s="2">
         <v>0.86</v>
       </c>
     </row>
-    <row r="100">
-      <c r="A100" t="n">
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="17.25">
+      <c r="A100" s="2">
         <v>0.1</v>
       </c>
-      <c r="B100" t="n">
+      <c r="B100" s="2">
         <v>3.16</v>
       </c>
-      <c r="C100" t="n">
+      <c r="C100" s="2">
         <v>0.92</v>
       </c>
-      <c r="D100" t="n">
+      <c r="D100" s="2">
         <v>0.97</v>
       </c>
     </row>
-    <row r="101">
-      <c r="A101" t="n">
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="17.25">
+      <c r="A101" s="2">
         <v>0.23</v>
       </c>
-      <c r="B101" t="n">
+      <c r="B101" s="2">
         <v>1.86</v>
       </c>
-      <c r="C101" t="n">
+      <c r="C101" s="2">
         <v>0.51</v>
       </c>
-      <c r="D101" t="n">
+      <c r="D101" s="2">
         <v>0.83</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>